<commit_message>
Ran analysis through 1-2.
</commit_message>
<xml_diff>
--- a/Results/2_jointAssociations.xlsx
+++ b/Results/2_jointAssociations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>outcomeVar</t>
   </si>
@@ -74,6 +74,306 @@
   </si>
   <si>
     <t>0.001 (-0.009, 0.011)</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>4530, 3096</t>
+  </si>
+  <si>
+    <t>-0.430 (-0.527, -0.333)**</t>
+  </si>
+  <si>
+    <t>-0.390 (-0.480, -0.300)**</t>
+  </si>
+  <si>
+    <t>-0.040 (-0.154, 0.073)</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>4530, 3096</t>
+  </si>
+  <si>
+    <t>-0.112 (-0.208, -0.016)*</t>
+  </si>
+  <si>
+    <t>-0.242 (-0.325, -0.160)**</t>
+  </si>
+  <si>
+    <t>0.130 (0.015, 0.245)*</t>
+  </si>
+  <si>
+    <t>mbpsys</t>
+  </si>
+  <si>
+    <t>5617, 3822</t>
+  </si>
+  <si>
+    <t>-0.055 (-0.064, -0.046)**</t>
+  </si>
+  <si>
+    <t>-0.012 (-0.022, -0.003)*</t>
+  </si>
+  <si>
+    <t>-0.043 (-0.054, -0.031)**</t>
+  </si>
+  <si>
+    <t>mbpsys</t>
+  </si>
+  <si>
+    <t>5617, 3822</t>
+  </si>
+  <si>
+    <t>-0.037 (-0.046, -0.028)**</t>
+  </si>
+  <si>
+    <t>-0.003 (-0.012, 0.007)</t>
+  </si>
+  <si>
+    <t>-0.034 (-0.046, -0.023)**</t>
+  </si>
+  <si>
+    <t>mbpdia</t>
+  </si>
+  <si>
+    <t>5629, 3834</t>
+  </si>
+  <si>
+    <t>-0.061 (-0.070, -0.051)**</t>
+  </si>
+  <si>
+    <t>-0.029 (-0.040, -0.018)**</t>
+  </si>
+  <si>
+    <t>-0.032 (-0.045, -0.019)**</t>
+  </si>
+  <si>
+    <t>mbpdia</t>
+  </si>
+  <si>
+    <t>5629, 3834</t>
+  </si>
+  <si>
+    <t>-0.028 (-0.038, -0.019)**</t>
+  </si>
+  <si>
+    <t>-0.011 (-0.021, -0.000)*</t>
+  </si>
+  <si>
+    <t>-0.017 (-0.030, -0.005)**</t>
+  </si>
+  <si>
+    <t>nefa</t>
+  </si>
+  <si>
+    <t>4521, 3086</t>
+  </si>
+  <si>
+    <t>-0.030 (-0.073, 0.012)</t>
+  </si>
+  <si>
+    <t>-0.082 (-0.135, -0.029)**</t>
+  </si>
+  <si>
+    <t>0.052 (-0.011, 0.114)</t>
+  </si>
+  <si>
+    <t>nefa</t>
+  </si>
+  <si>
+    <t>4521, 3086</t>
+  </si>
+  <si>
+    <t>-0.008 (-0.051, 0.036)</t>
+  </si>
+  <si>
+    <t>-0.069 (-0.122, -0.016)*</t>
+  </si>
+  <si>
+    <t>0.062 (-0.001, 0.124)</t>
+  </si>
+  <si>
+    <t>leptin</t>
+  </si>
+  <si>
+    <t>4523, 3084</t>
+  </si>
+  <si>
+    <t>-0.843 (-0.954, -0.733)**</t>
+  </si>
+  <si>
+    <t>-0.624 (-0.736, -0.511)**</t>
+  </si>
+  <si>
+    <t>-0.220 (-0.356, -0.084)**</t>
+  </si>
+  <si>
+    <t>leptin</t>
+  </si>
+  <si>
+    <t>4523, 3084</t>
+  </si>
+  <si>
+    <t>-0.245 (-0.319, -0.172)**</t>
+  </si>
+  <si>
+    <t>-0.335 (-0.425, -0.245)**</t>
+  </si>
+  <si>
+    <t>0.090 (-0.008, 0.188)</t>
+  </si>
+  <si>
+    <t>adiponectin</t>
+  </si>
+  <si>
+    <t>4523, 3089</t>
+  </si>
+  <si>
+    <t>0.129 (0.094, 0.164)**</t>
+  </si>
+  <si>
+    <t>0.108 (0.061, 0.154)**</t>
+  </si>
+  <si>
+    <t>0.021 (-0.031, 0.073)</t>
+  </si>
+  <si>
+    <t>adiponectin</t>
+  </si>
+  <si>
+    <t>4523, 3089</t>
+  </si>
+  <si>
+    <t>0.029 (-0.008, 0.067)</t>
+  </si>
+  <si>
+    <t>0.052 (0.006, 0.099)*</t>
+  </si>
+  <si>
+    <t>-0.023 (-0.075, 0.029)</t>
+  </si>
+  <si>
+    <t>crp</t>
+  </si>
+  <si>
+    <t>4409, 3034</t>
+  </si>
+  <si>
+    <t>-0.947 (-1.493, -0.402)**</t>
+  </si>
+  <si>
+    <t>-0.420 (-0.707, -0.134)**</t>
+  </si>
+  <si>
+    <t>-0.527 (-1.216, 0.162)</t>
+  </si>
+  <si>
+    <t>crp</t>
+  </si>
+  <si>
+    <t>4409, 3034</t>
+  </si>
+  <si>
+    <t>-0.664 (-1.159, -0.169)**</t>
+  </si>
+  <si>
+    <t>-0.222 (-0.576, 0.132)</t>
+  </si>
+  <si>
+    <t>-0.442 (-1.193, 0.308)</t>
+  </si>
+  <si>
+    <t>ldl</t>
+  </si>
+  <si>
+    <t>5623, 3781</t>
+  </si>
+  <si>
+    <t>-0.051 (-0.071, -0.031)**</t>
+  </si>
+  <si>
+    <t>0.019 (-0.002, 0.041)</t>
+  </si>
+  <si>
+    <t>-0.070 (-0.097, -0.044)**</t>
+  </si>
+  <si>
+    <t>ldl</t>
+  </si>
+  <si>
+    <t>5623, 3781</t>
+  </si>
+  <si>
+    <t>-0.025 (-0.045, -0.006)*</t>
+  </si>
+  <si>
+    <t>0.034 (0.012, 0.056)**</t>
+  </si>
+  <si>
+    <t>-0.059 (-0.086, -0.033)**</t>
+  </si>
+  <si>
+    <t>hdl</t>
+  </si>
+  <si>
+    <t>5636, 3835</t>
+  </si>
+  <si>
+    <t>0.091 (0.074, 0.108)**</t>
+  </si>
+  <si>
+    <t>0.116 (0.095, 0.137)**</t>
+  </si>
+  <si>
+    <t>-0.025 (-0.049, -0.001)*</t>
+  </si>
+  <si>
+    <t>hdl</t>
+  </si>
+  <si>
+    <t>5636, 3835</t>
+  </si>
+  <si>
+    <t>0.033 (0.016, 0.050)**</t>
+  </si>
+  <si>
+    <t>0.083 (0.063, 0.104)**</t>
+  </si>
+  <si>
+    <t>-0.050 (-0.074, -0.026)**</t>
+  </si>
+  <si>
+    <t>glucose0</t>
+  </si>
+  <si>
+    <t>5615, 3836</t>
+  </si>
+  <si>
+    <t>-0.034 (-0.043, -0.025)**</t>
+  </si>
+  <si>
+    <t>-0.020 (-0.031, -0.008)**</t>
+  </si>
+  <si>
+    <t>-0.014 (-0.028, -0.001)*</t>
+  </si>
+  <si>
+    <t>glucose0</t>
+  </si>
+  <si>
+    <t>5615, 3836</t>
+  </si>
+  <si>
+    <t>-0.010 (-0.019, -0.001)*</t>
+  </si>
+  <si>
+    <t>-0.007 (-0.018, 0.005)</t>
+  </si>
+  <si>
+    <t>-0.004 (-0.017, 0.010)</t>
   </si>
 </sst>
 </file>
@@ -117,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -152,6 +452,176 @@
       </c>
       <c r="E2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -160,7 +630,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E12"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -197,6 +667,176 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>